<commit_message>
kiểm tra không có  dữ liệu thêm
</commit_message>
<xml_diff>
--- a/public/insert_template/themsp.xlsx
+++ b/public/insert_template/themsp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\PHP\quanlycuahang\public\insert_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D251BA37-76A4-4E38-B5EF-A9333C1C71D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4F917B-F5AB-40EA-9029-390EF0A55DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5868" yWindow="564" windowWidth="17172" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -489,11 +489,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -621,496 +621,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K102">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>